<commit_message>
Update controlled vocabulary ```
</commit_message>
<xml_diff>
--- a/STAC/data/vocab.xlsx
+++ b/STAC/data/vocab.xlsx
@@ -385,7 +385,7 @@
     <t>float32</t>
   </si>
   <si>
-    <t>|S##</t>
+    <t>string</t>
   </si>
   <si>
     <t>int8</t>
@@ -397,7 +397,7 @@
     <t>['esl_gwl']</t>
   </si>
   <si>
-    <t>['shore_mon_fut', 'shore_mon', 'shore_mon_hr']</t>
+    <t>['shore_mon_hr', 'shore_mon_fut', 'shore_mon']</t>
   </si>
   <si>
     <t>['shore_mon_hr']</t>
@@ -406,16 +406,16 @@
     <t>['shore_mon']</t>
   </si>
   <si>
-    <t>['world_gdp', 'shore_mon_fut', 'shore_mon_drivers', 'world_pop', 'shore_mon', 'sed_class']</t>
-  </si>
-  <si>
-    <t>['shore_mon_drivers', 'shore_mon_fut', 'shore_mon']</t>
-  </si>
-  <si>
-    <t>['shore_mon_drivers', 'shore_mon_hr']</t>
-  </si>
-  <si>
-    <t>['world_gdp', 'shore_mon_fut', 'shore_mon_drivers', 'world_pop', 'shore_mon', 'shore_mon_hr', 'sed_class']</t>
+    <t>['sed_class', 'shore_mon', 'world_pop', 'shore_mon_drivers', 'shore_mon_fut', 'world_gdp']</t>
+  </si>
+  <si>
+    <t>['shore_mon_fut', 'shore_mon_drivers', 'shore_mon']</t>
+  </si>
+  <si>
+    <t>['shore_mon_hr', 'shore_mon_drivers']</t>
+  </si>
+  <si>
+    <t>['sed_class', 'shore_mon_hr', 'shore_mon', 'world_pop', 'shore_mon_drivers', 'shore_mon_fut', 'world_gdp']</t>
   </si>
   <si>
     <t>['shore_mon_drivers']</t>
@@ -427,7 +427,7 @@
     <t>['shore_mon_fut']</t>
   </si>
   <si>
-    <t>['shore_mon', 'shore_mon_hr']</t>
+    <t>['shore_mon_hr', 'shore_mon']</t>
   </si>
   <si>
     <t>['world_pop']</t>
@@ -502,10 +502,10 @@
     <t>[21.0]</t>
   </si>
   <si>
-    <t>[b'LINESTRING (47.885022 29.319149, 47.879413 29.33403)', b'LINESTRING (-74.382468591 -50.3791437735, -74.3917820288 -50.3889403594)', b'LINESTRING (-71.624166 10.990024, -71.60742 10.996413)', b'LINESTRING (-74.3863095545 -50.3776589451, -74.39562299239999 -50.3874558377)', b'LINESTRING (-72.98252423386046 -54.45955389684386, -72.99521062694167 -54.448286932134025)']</t>
-  </si>
-  <si>
-    <t>[b'BOX_028_183_0', b'BOX_028_000_0', b'BOX_145_168_39', b'BOX_117_067_110', b'BOX_028_183_1']</t>
+    <t>[b'LINESTRING (-72.98252423386046 -54.45955389684386, -72.99521062694167 -54.448286932134025)', b'LINESTRING (-74.3863095545 -50.3776589451, -74.39562299239999 -50.3874558377)', b'LINESTRING (-71.624166 10.990024, -71.60742 10.996413)', b'LINESTRING (47.885022 29.319149, 47.879413 29.33403)', b'LINESTRING (-74.382468591 -50.3791437735, -74.3917820288 -50.3889403594)']</t>
+  </si>
+  <si>
+    <t>[b'BOX_028_183_1', b'BOX_028_183_0', b'BOX_028_000_0', b'BOX_117_067_110', b'BOX_145_168_39']</t>
   </si>
   <si>
     <t>[3.436772245547764, 6.9373716882311545, 14.088575593402023]</t>

</xml_diff>